<commit_message>
risucito ad aggiornare "dinamicamente" la data al foglio, ma non è perpetua, da sistemare il raggruppamento in settimane
</commit_message>
<xml_diff>
--- a/windows_form_app/TEST_CALENDAR_EXCEL_WEEK.xlsx
+++ b/windows_form_app/TEST_CALENDAR_EXCEL_WEEK.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R1a43ebb660fc488b"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R9b528f7613d849a1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -20,325 +20,325 @@
     <x:t>W 1</x:t>
   </x:si>
   <x:si>
-    <x:t>22/3/2019</x:t>
+    <x:t>23/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 2</x:t>
   </x:si>
   <x:si>
-    <x:t>23/3/2019</x:t>
+    <x:t>24/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 3</x:t>
   </x:si>
   <x:si>
-    <x:t>24/3/2019</x:t>
+    <x:t>25/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 4</x:t>
   </x:si>
   <x:si>
-    <x:t>25/3/2019</x:t>
+    <x:t>26/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 5</x:t>
   </x:si>
   <x:si>
-    <x:t>26/3/2019</x:t>
+    <x:t>27/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 6</x:t>
   </x:si>
   <x:si>
-    <x:t>27/3/2019</x:t>
+    <x:t>28/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 7</x:t>
   </x:si>
   <x:si>
-    <x:t>28/3/2019</x:t>
+    <x:t>29/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 8</x:t>
   </x:si>
   <x:si>
-    <x:t>29/3/2019</x:t>
+    <x:t>30/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 9</x:t>
   </x:si>
   <x:si>
-    <x:t>30/3/2019</x:t>
+    <x:t>31/3/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 10</x:t>
   </x:si>
   <x:si>
-    <x:t>31/3/2019</x:t>
+    <x:t>1/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 11</x:t>
   </x:si>
   <x:si>
-    <x:t>32/3/2019</x:t>
+    <x:t>2/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 12</x:t>
   </x:si>
   <x:si>
-    <x:t>33/3/2019</x:t>
+    <x:t>3/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 13</x:t>
   </x:si>
   <x:si>
-    <x:t>34/3/2019</x:t>
+    <x:t>4/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 14</x:t>
   </x:si>
   <x:si>
-    <x:t>35/3/2019</x:t>
+    <x:t>5/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 15</x:t>
   </x:si>
   <x:si>
-    <x:t>36/3/2019</x:t>
+    <x:t>6/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 16</x:t>
   </x:si>
   <x:si>
-    <x:t>37/3/2019</x:t>
+    <x:t>7/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 17</x:t>
   </x:si>
   <x:si>
-    <x:t>38/3/2019</x:t>
+    <x:t>8/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 18</x:t>
   </x:si>
   <x:si>
-    <x:t>39/3/2019</x:t>
+    <x:t>9/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 19</x:t>
   </x:si>
   <x:si>
-    <x:t>40/3/2019</x:t>
+    <x:t>10/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 20</x:t>
   </x:si>
   <x:si>
-    <x:t>41/3/2019</x:t>
+    <x:t>11/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 21</x:t>
   </x:si>
   <x:si>
-    <x:t>42/3/2019</x:t>
+    <x:t>12/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 22</x:t>
   </x:si>
   <x:si>
-    <x:t>43/3/2019</x:t>
+    <x:t>13/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 23</x:t>
   </x:si>
   <x:si>
-    <x:t>44/3/2019</x:t>
+    <x:t>14/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 24</x:t>
   </x:si>
   <x:si>
-    <x:t>45/3/2019</x:t>
+    <x:t>15/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 25</x:t>
   </x:si>
   <x:si>
-    <x:t>46/3/2019</x:t>
+    <x:t>16/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 26</x:t>
   </x:si>
   <x:si>
-    <x:t>47/3/2019</x:t>
+    <x:t>17/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 27</x:t>
   </x:si>
   <x:si>
-    <x:t>48/3/2019</x:t>
+    <x:t>18/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 28</x:t>
   </x:si>
   <x:si>
-    <x:t>49/3/2019</x:t>
+    <x:t>19/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 29</x:t>
   </x:si>
   <x:si>
-    <x:t>50/3/2019</x:t>
+    <x:t>20/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 30</x:t>
   </x:si>
   <x:si>
-    <x:t>51/3/2019</x:t>
+    <x:t>21/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 31</x:t>
   </x:si>
   <x:si>
-    <x:t>52/3/2019</x:t>
+    <x:t>22/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 32</x:t>
   </x:si>
   <x:si>
-    <x:t>53/3/2019</x:t>
+    <x:t>23/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 33</x:t>
   </x:si>
   <x:si>
-    <x:t>54/3/2019</x:t>
+    <x:t>24/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 34</x:t>
   </x:si>
   <x:si>
-    <x:t>55/3/2019</x:t>
+    <x:t>25/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 35</x:t>
   </x:si>
   <x:si>
-    <x:t>56/3/2019</x:t>
+    <x:t>26/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 36</x:t>
   </x:si>
   <x:si>
-    <x:t>57/3/2019</x:t>
+    <x:t>27/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 37</x:t>
   </x:si>
   <x:si>
-    <x:t>58/3/2019</x:t>
+    <x:t>28/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 38</x:t>
   </x:si>
   <x:si>
-    <x:t>59/3/2019</x:t>
+    <x:t>29/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 39</x:t>
   </x:si>
   <x:si>
-    <x:t>60/3/2019</x:t>
+    <x:t>30/4/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 40</x:t>
   </x:si>
   <x:si>
-    <x:t>61/3/2019</x:t>
+    <x:t>1/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 41</x:t>
   </x:si>
   <x:si>
-    <x:t>62/3/2019</x:t>
+    <x:t>2/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 42</x:t>
   </x:si>
   <x:si>
-    <x:t>63/3/2019</x:t>
+    <x:t>3/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 43</x:t>
   </x:si>
   <x:si>
-    <x:t>64/3/2019</x:t>
+    <x:t>4/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 44</x:t>
   </x:si>
   <x:si>
-    <x:t>65/3/2019</x:t>
+    <x:t>5/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 45</x:t>
   </x:si>
   <x:si>
-    <x:t>66/3/2019</x:t>
+    <x:t>6/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 46</x:t>
   </x:si>
   <x:si>
-    <x:t>67/3/2019</x:t>
+    <x:t>7/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 47</x:t>
   </x:si>
   <x:si>
-    <x:t>68/3/2019</x:t>
+    <x:t>8/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 48</x:t>
   </x:si>
   <x:si>
-    <x:t>69/3/2019</x:t>
+    <x:t>9/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 49</x:t>
   </x:si>
   <x:si>
-    <x:t>70/3/2019</x:t>
+    <x:t>10/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 50</x:t>
   </x:si>
   <x:si>
-    <x:t>71/3/2019</x:t>
+    <x:t>11/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 51</x:t>
   </x:si>
   <x:si>
-    <x:t>72/3/2019</x:t>
+    <x:t>12/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 52</x:t>
   </x:si>
   <x:si>
-    <x:t>73/3/2019</x:t>
+    <x:t>13/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 53</x:t>
   </x:si>
   <x:si>
-    <x:t>74/3/2019</x:t>
+    <x:t>14/5/2019</x:t>
   </x:si>
   <x:si>
     <x:t>W 54</x:t>
   </x:si>
   <x:si>
-    <x:t>75/3/2019</x:t>
+    <x:t>15/5/2019</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -678,7 +678,7 @@
 
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:BB1370"/>
+  <x:dimension ref="A1:BB3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -1087,378 +1087,11 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="371">
-    <x:mergeCell ref="B10:H10"/>
-    <x:mergeCell ref="B11:H11"/>
-    <x:mergeCell ref="B12:H12"/>
-    <x:mergeCell ref="B13:H13"/>
-    <x:mergeCell ref="B14:H14"/>
-    <x:mergeCell ref="B15:H15"/>
-    <x:mergeCell ref="B16:H16"/>
-    <x:mergeCell ref="B17:H17"/>
-    <x:mergeCell ref="B18:H18"/>
-    <x:mergeCell ref="B19:H19"/>
-    <x:mergeCell ref="B110:H110"/>
-    <x:mergeCell ref="B111:H111"/>
-    <x:mergeCell ref="B112:H112"/>
-    <x:mergeCell ref="B113:H113"/>
-    <x:mergeCell ref="B114:H114"/>
-    <x:mergeCell ref="B115:H115"/>
-    <x:mergeCell ref="B116:H116"/>
-    <x:mergeCell ref="B117:H117"/>
-    <x:mergeCell ref="B118:H118"/>
-    <x:mergeCell ref="B119:H119"/>
-    <x:mergeCell ref="B120:H120"/>
-    <x:mergeCell ref="B121:H121"/>
-    <x:mergeCell ref="B122:H122"/>
-    <x:mergeCell ref="B123:H123"/>
-    <x:mergeCell ref="B124:H124"/>
-    <x:mergeCell ref="B125:H125"/>
-    <x:mergeCell ref="B126:H126"/>
-    <x:mergeCell ref="B127:H127"/>
-    <x:mergeCell ref="B128:H128"/>
-    <x:mergeCell ref="B129:H129"/>
-    <x:mergeCell ref="B130:H130"/>
-    <x:mergeCell ref="B131:H131"/>
-    <x:mergeCell ref="B132:H132"/>
-    <x:mergeCell ref="B133:H133"/>
-    <x:mergeCell ref="B134:H134"/>
-    <x:mergeCell ref="B135:H135"/>
-    <x:mergeCell ref="B136:H136"/>
-    <x:mergeCell ref="B137:H137"/>
-    <x:mergeCell ref="B138:H138"/>
-    <x:mergeCell ref="B139:H139"/>
-    <x:mergeCell ref="B140:H140"/>
-    <x:mergeCell ref="B141:H141"/>
-    <x:mergeCell ref="B142:H142"/>
-    <x:mergeCell ref="B143:H143"/>
-    <x:mergeCell ref="B144:H144"/>
-    <x:mergeCell ref="B145:H145"/>
-    <x:mergeCell ref="B146:H146"/>
-    <x:mergeCell ref="B147:H147"/>
-    <x:mergeCell ref="B148:H148"/>
-    <x:mergeCell ref="B149:H149"/>
-    <x:mergeCell ref="B150:H150"/>
-    <x:mergeCell ref="B151:H151"/>
-    <x:mergeCell ref="B152:H152"/>
-    <x:mergeCell ref="B153:H153"/>
-    <x:mergeCell ref="B154:H154"/>
-    <x:mergeCell ref="B155:H155"/>
-    <x:mergeCell ref="B156:H156"/>
-    <x:mergeCell ref="B157:H157"/>
-    <x:mergeCell ref="B158:H158"/>
-    <x:mergeCell ref="B159:H159"/>
-    <x:mergeCell ref="B160:H160"/>
-    <x:mergeCell ref="B161:H161"/>
-    <x:mergeCell ref="B162:H162"/>
-    <x:mergeCell ref="B163:H163"/>
-    <x:mergeCell ref="B164:H164"/>
-    <x:mergeCell ref="B165:H165"/>
-    <x:mergeCell ref="B166:H166"/>
-    <x:mergeCell ref="B167:H167"/>
-    <x:mergeCell ref="B168:H168"/>
-    <x:mergeCell ref="B169:H169"/>
-    <x:mergeCell ref="B170:H170"/>
-    <x:mergeCell ref="B171:H171"/>
-    <x:mergeCell ref="B172:H172"/>
-    <x:mergeCell ref="B173:H173"/>
-    <x:mergeCell ref="B174:H174"/>
-    <x:mergeCell ref="B175:H175"/>
-    <x:mergeCell ref="B176:H176"/>
-    <x:mergeCell ref="B177:H177"/>
-    <x:mergeCell ref="B178:H178"/>
-    <x:mergeCell ref="B179:H179"/>
-    <x:mergeCell ref="B180:H180"/>
-    <x:mergeCell ref="B181:H181"/>
-    <x:mergeCell ref="B182:H182"/>
-    <x:mergeCell ref="B183:H183"/>
-    <x:mergeCell ref="B184:H184"/>
-    <x:mergeCell ref="B185:H185"/>
-    <x:mergeCell ref="B186:H186"/>
-    <x:mergeCell ref="B187:H187"/>
-    <x:mergeCell ref="B188:H188"/>
-    <x:mergeCell ref="B189:H189"/>
-    <x:mergeCell ref="B190:H190"/>
-    <x:mergeCell ref="B191:H191"/>
-    <x:mergeCell ref="B192:H192"/>
-    <x:mergeCell ref="B193:H193"/>
-    <x:mergeCell ref="B194:H194"/>
-    <x:mergeCell ref="B195:H195"/>
-    <x:mergeCell ref="B196:H196"/>
-    <x:mergeCell ref="B197:H197"/>
-    <x:mergeCell ref="B198:H198"/>
-    <x:mergeCell ref="B199:H199"/>
-    <x:mergeCell ref="B1100:H1100"/>
-    <x:mergeCell ref="B1101:H1101"/>
-    <x:mergeCell ref="B1102:H1102"/>
-    <x:mergeCell ref="B1103:H1103"/>
-    <x:mergeCell ref="B1104:H1104"/>
-    <x:mergeCell ref="B1105:H1105"/>
-    <x:mergeCell ref="B1106:H1106"/>
-    <x:mergeCell ref="B1107:H1107"/>
-    <x:mergeCell ref="B1108:H1108"/>
-    <x:mergeCell ref="B1109:H1109"/>
-    <x:mergeCell ref="B1110:H1110"/>
-    <x:mergeCell ref="B1111:H1111"/>
-    <x:mergeCell ref="B1112:H1112"/>
-    <x:mergeCell ref="B1113:H1113"/>
-    <x:mergeCell ref="B1114:H1114"/>
-    <x:mergeCell ref="B1115:H1115"/>
-    <x:mergeCell ref="B1116:H1116"/>
-    <x:mergeCell ref="B1117:H1117"/>
-    <x:mergeCell ref="B1118:H1118"/>
-    <x:mergeCell ref="B1119:H1119"/>
-    <x:mergeCell ref="B1120:H1120"/>
-    <x:mergeCell ref="B1121:H1121"/>
-    <x:mergeCell ref="B1122:H1122"/>
-    <x:mergeCell ref="B1123:H1123"/>
-    <x:mergeCell ref="B1124:H1124"/>
-    <x:mergeCell ref="B1125:H1125"/>
-    <x:mergeCell ref="B1126:H1126"/>
-    <x:mergeCell ref="B1127:H1127"/>
-    <x:mergeCell ref="B1128:H1128"/>
-    <x:mergeCell ref="B1129:H1129"/>
-    <x:mergeCell ref="B1130:H1130"/>
-    <x:mergeCell ref="B1131:H1131"/>
-    <x:mergeCell ref="B1132:H1132"/>
-    <x:mergeCell ref="B1133:H1133"/>
-    <x:mergeCell ref="B1134:H1134"/>
-    <x:mergeCell ref="B1135:H1135"/>
-    <x:mergeCell ref="B1136:H1136"/>
-    <x:mergeCell ref="B1137:H1137"/>
-    <x:mergeCell ref="B1138:H1138"/>
-    <x:mergeCell ref="B1139:H1139"/>
-    <x:mergeCell ref="B1140:H1140"/>
-    <x:mergeCell ref="B1141:H1141"/>
-    <x:mergeCell ref="B1142:H1142"/>
-    <x:mergeCell ref="B1143:H1143"/>
-    <x:mergeCell ref="B1144:H1144"/>
-    <x:mergeCell ref="B1145:H1145"/>
-    <x:mergeCell ref="B1146:H1146"/>
-    <x:mergeCell ref="B1147:H1147"/>
-    <x:mergeCell ref="B1148:H1148"/>
-    <x:mergeCell ref="B1149:H1149"/>
-    <x:mergeCell ref="B1150:H1150"/>
-    <x:mergeCell ref="B1151:H1151"/>
-    <x:mergeCell ref="B1152:H1152"/>
-    <x:mergeCell ref="B1153:H1153"/>
-    <x:mergeCell ref="B1154:H1154"/>
-    <x:mergeCell ref="B1155:H1155"/>
-    <x:mergeCell ref="B1156:H1156"/>
-    <x:mergeCell ref="B1157:H1157"/>
-    <x:mergeCell ref="B1158:H1158"/>
-    <x:mergeCell ref="B1159:H1159"/>
-    <x:mergeCell ref="B1160:H1160"/>
-    <x:mergeCell ref="B1161:H1161"/>
-    <x:mergeCell ref="B1162:H1162"/>
-    <x:mergeCell ref="B1163:H1163"/>
-    <x:mergeCell ref="B1164:H1164"/>
-    <x:mergeCell ref="B1165:H1165"/>
-    <x:mergeCell ref="B1166:H1166"/>
-    <x:mergeCell ref="B1167:H1167"/>
-    <x:mergeCell ref="B1168:H1168"/>
-    <x:mergeCell ref="B1169:H1169"/>
-    <x:mergeCell ref="B1170:H1170"/>
-    <x:mergeCell ref="B1171:H1171"/>
-    <x:mergeCell ref="B1172:H1172"/>
-    <x:mergeCell ref="B1173:H1173"/>
-    <x:mergeCell ref="B1174:H1174"/>
-    <x:mergeCell ref="B1175:H1175"/>
-    <x:mergeCell ref="B1176:H1176"/>
-    <x:mergeCell ref="B1177:H1177"/>
-    <x:mergeCell ref="B1178:H1178"/>
-    <x:mergeCell ref="B1179:H1179"/>
-    <x:mergeCell ref="B1180:H1180"/>
-    <x:mergeCell ref="B1181:H1181"/>
-    <x:mergeCell ref="B1182:H1182"/>
-    <x:mergeCell ref="B1183:H1183"/>
-    <x:mergeCell ref="B1184:H1184"/>
-    <x:mergeCell ref="B1185:H1185"/>
-    <x:mergeCell ref="B1186:H1186"/>
-    <x:mergeCell ref="B1187:H1187"/>
-    <x:mergeCell ref="B1188:H1188"/>
-    <x:mergeCell ref="B1189:H1189"/>
-    <x:mergeCell ref="B1190:H1190"/>
-    <x:mergeCell ref="B1191:H1191"/>
-    <x:mergeCell ref="B1192:H1192"/>
-    <x:mergeCell ref="B1193:H1193"/>
-    <x:mergeCell ref="B1194:H1194"/>
-    <x:mergeCell ref="B1195:H1195"/>
-    <x:mergeCell ref="B1196:H1196"/>
-    <x:mergeCell ref="B1197:H1197"/>
-    <x:mergeCell ref="B1198:H1198"/>
-    <x:mergeCell ref="B1199:H1199"/>
-    <x:mergeCell ref="B1200:H1200"/>
-    <x:mergeCell ref="B1201:H1201"/>
-    <x:mergeCell ref="B1202:H1202"/>
-    <x:mergeCell ref="B1203:H1203"/>
-    <x:mergeCell ref="B1204:H1204"/>
-    <x:mergeCell ref="B1205:H1205"/>
-    <x:mergeCell ref="B1206:H1206"/>
-    <x:mergeCell ref="B1207:H1207"/>
-    <x:mergeCell ref="B1208:H1208"/>
-    <x:mergeCell ref="B1209:H1209"/>
-    <x:mergeCell ref="B1210:H1210"/>
-    <x:mergeCell ref="B1211:H1211"/>
-    <x:mergeCell ref="B1212:H1212"/>
-    <x:mergeCell ref="B1213:H1213"/>
-    <x:mergeCell ref="B1214:H1214"/>
-    <x:mergeCell ref="B1215:H1215"/>
-    <x:mergeCell ref="B1216:H1216"/>
-    <x:mergeCell ref="B1217:H1217"/>
-    <x:mergeCell ref="B1218:H1218"/>
-    <x:mergeCell ref="B1219:H1219"/>
-    <x:mergeCell ref="B1220:H1220"/>
-    <x:mergeCell ref="B1221:H1221"/>
-    <x:mergeCell ref="B1222:H1222"/>
-    <x:mergeCell ref="B1223:H1223"/>
-    <x:mergeCell ref="B1224:H1224"/>
-    <x:mergeCell ref="B1225:H1225"/>
-    <x:mergeCell ref="B1226:H1226"/>
-    <x:mergeCell ref="B1227:H1227"/>
-    <x:mergeCell ref="B1228:H1228"/>
-    <x:mergeCell ref="B1229:H1229"/>
-    <x:mergeCell ref="B1230:H1230"/>
-    <x:mergeCell ref="B1231:H1231"/>
-    <x:mergeCell ref="B1232:H1232"/>
-    <x:mergeCell ref="B1233:H1233"/>
-    <x:mergeCell ref="B1234:H1234"/>
-    <x:mergeCell ref="B1235:H1235"/>
-    <x:mergeCell ref="B1236:H1236"/>
-    <x:mergeCell ref="B1237:H1237"/>
-    <x:mergeCell ref="B1238:H1238"/>
-    <x:mergeCell ref="B1239:H1239"/>
-    <x:mergeCell ref="B1240:H1240"/>
-    <x:mergeCell ref="B1241:H1241"/>
-    <x:mergeCell ref="B1242:H1242"/>
-    <x:mergeCell ref="B1243:H1243"/>
-    <x:mergeCell ref="B1244:H1244"/>
-    <x:mergeCell ref="B1245:H1245"/>
-    <x:mergeCell ref="B1246:H1246"/>
-    <x:mergeCell ref="B1247:H1247"/>
-    <x:mergeCell ref="B1248:H1248"/>
-    <x:mergeCell ref="B1249:H1249"/>
-    <x:mergeCell ref="B1250:H1250"/>
-    <x:mergeCell ref="B1251:H1251"/>
-    <x:mergeCell ref="B1252:H1252"/>
-    <x:mergeCell ref="B1253:H1253"/>
-    <x:mergeCell ref="B1254:H1254"/>
-    <x:mergeCell ref="B1255:H1255"/>
-    <x:mergeCell ref="B1256:H1256"/>
-    <x:mergeCell ref="B1257:H1257"/>
-    <x:mergeCell ref="B1258:H1258"/>
-    <x:mergeCell ref="B1259:H1259"/>
-    <x:mergeCell ref="B1260:H1260"/>
-    <x:mergeCell ref="B1261:H1261"/>
-    <x:mergeCell ref="B1262:H1262"/>
-    <x:mergeCell ref="B1263:H1263"/>
-    <x:mergeCell ref="B1264:H1264"/>
-    <x:mergeCell ref="B1265:H1265"/>
-    <x:mergeCell ref="B1266:H1266"/>
-    <x:mergeCell ref="B1267:H1267"/>
-    <x:mergeCell ref="B1268:H1268"/>
-    <x:mergeCell ref="B1269:H1269"/>
-    <x:mergeCell ref="B1270:H1270"/>
-    <x:mergeCell ref="B1271:H1271"/>
-    <x:mergeCell ref="B1272:H1272"/>
-    <x:mergeCell ref="B1273:H1273"/>
-    <x:mergeCell ref="B1274:H1274"/>
-    <x:mergeCell ref="B1275:H1275"/>
-    <x:mergeCell ref="B1276:H1276"/>
-    <x:mergeCell ref="B1277:H1277"/>
-    <x:mergeCell ref="B1278:H1278"/>
-    <x:mergeCell ref="B1279:H1279"/>
-    <x:mergeCell ref="B1280:H1280"/>
-    <x:mergeCell ref="B1281:H1281"/>
-    <x:mergeCell ref="B1282:H1282"/>
-    <x:mergeCell ref="B1283:H1283"/>
-    <x:mergeCell ref="B1284:H1284"/>
-    <x:mergeCell ref="B1285:H1285"/>
-    <x:mergeCell ref="B1286:H1286"/>
-    <x:mergeCell ref="B1287:H1287"/>
-    <x:mergeCell ref="B1288:H1288"/>
-    <x:mergeCell ref="B1289:H1289"/>
-    <x:mergeCell ref="B1290:H1290"/>
-    <x:mergeCell ref="B1291:H1291"/>
-    <x:mergeCell ref="B1292:H1292"/>
-    <x:mergeCell ref="B1293:H1293"/>
-    <x:mergeCell ref="B1294:H1294"/>
-    <x:mergeCell ref="B1295:H1295"/>
-    <x:mergeCell ref="B1296:H1296"/>
-    <x:mergeCell ref="B1297:H1297"/>
-    <x:mergeCell ref="B1298:H1298"/>
-    <x:mergeCell ref="B1299:H1299"/>
-    <x:mergeCell ref="B1300:H1300"/>
-    <x:mergeCell ref="B1301:H1301"/>
-    <x:mergeCell ref="B1302:H1302"/>
-    <x:mergeCell ref="B1303:H1303"/>
-    <x:mergeCell ref="B1304:H1304"/>
-    <x:mergeCell ref="B1305:H1305"/>
-    <x:mergeCell ref="B1306:H1306"/>
-    <x:mergeCell ref="B1307:H1307"/>
-    <x:mergeCell ref="B1308:H1308"/>
-    <x:mergeCell ref="B1309:H1309"/>
-    <x:mergeCell ref="B1310:H1310"/>
-    <x:mergeCell ref="B1311:H1311"/>
-    <x:mergeCell ref="B1312:H1312"/>
-    <x:mergeCell ref="B1313:H1313"/>
-    <x:mergeCell ref="B1314:H1314"/>
-    <x:mergeCell ref="B1315:H1315"/>
-    <x:mergeCell ref="B1316:H1316"/>
-    <x:mergeCell ref="B1317:H1317"/>
-    <x:mergeCell ref="B1318:H1318"/>
-    <x:mergeCell ref="B1319:H1319"/>
-    <x:mergeCell ref="B1320:H1320"/>
-    <x:mergeCell ref="B1321:H1321"/>
-    <x:mergeCell ref="B1322:H1322"/>
-    <x:mergeCell ref="B1323:H1323"/>
-    <x:mergeCell ref="B1324:H1324"/>
-    <x:mergeCell ref="B1325:H1325"/>
-    <x:mergeCell ref="B1326:H1326"/>
-    <x:mergeCell ref="B1327:H1327"/>
-    <x:mergeCell ref="B1328:H1328"/>
-    <x:mergeCell ref="B1329:H1329"/>
-    <x:mergeCell ref="B1330:H1330"/>
-    <x:mergeCell ref="B1331:H1331"/>
-    <x:mergeCell ref="B1332:H1332"/>
-    <x:mergeCell ref="B1333:H1333"/>
-    <x:mergeCell ref="B1334:H1334"/>
-    <x:mergeCell ref="B1335:H1335"/>
-    <x:mergeCell ref="B1336:H1336"/>
-    <x:mergeCell ref="B1337:H1337"/>
-    <x:mergeCell ref="B1338:H1338"/>
-    <x:mergeCell ref="B1339:H1339"/>
-    <x:mergeCell ref="B1340:H1340"/>
-    <x:mergeCell ref="B1341:H1341"/>
-    <x:mergeCell ref="B1342:H1342"/>
-    <x:mergeCell ref="B1343:H1343"/>
-    <x:mergeCell ref="B1344:H1344"/>
-    <x:mergeCell ref="B1345:H1345"/>
-    <x:mergeCell ref="B1346:H1346"/>
-    <x:mergeCell ref="B1347:H1347"/>
-    <x:mergeCell ref="B1348:H1348"/>
-    <x:mergeCell ref="B1349:H1349"/>
-    <x:mergeCell ref="B1350:H1350"/>
-    <x:mergeCell ref="B1351:H1351"/>
-    <x:mergeCell ref="B1352:H1352"/>
-    <x:mergeCell ref="B1353:H1353"/>
-    <x:mergeCell ref="B1354:H1354"/>
-    <x:mergeCell ref="B1355:H1355"/>
-    <x:mergeCell ref="B1356:H1356"/>
-    <x:mergeCell ref="B1357:H1357"/>
-    <x:mergeCell ref="B1358:H1358"/>
-    <x:mergeCell ref="B1359:H1359"/>
-    <x:mergeCell ref="B1360:H1360"/>
-    <x:mergeCell ref="B1361:H1361"/>
-    <x:mergeCell ref="B1362:H1362"/>
-    <x:mergeCell ref="B1363:H1363"/>
-    <x:mergeCell ref="B1364:H1364"/>
-    <x:mergeCell ref="B1365:H1365"/>
-    <x:mergeCell ref="B1366:H1366"/>
-    <x:mergeCell ref="B1367:H1367"/>
-    <x:mergeCell ref="B1368:H1368"/>
-    <x:mergeCell ref="B1369:H1369"/>
-    <x:mergeCell ref="B1370:H1370"/>
+  <x:mergeCells count="4">
+    <x:mergeCell ref="B1:H1"/>
+    <x:mergeCell ref="I1:O1"/>
+    <x:mergeCell ref="P1:X1"/>
+    <x:mergeCell ref="Y1:AF1"/>
   </x:mergeCells>
 </x:worksheet>
 </file>
</xml_diff>